<commit_message>
Final draft of intrusion paper
</commit_message>
<xml_diff>
--- a/analysis/models/R/experiment_1/output/collated_experiment_1_fits.xlsx
+++ b/analysis/models/R/experiment_1/output/collated_experiment_1_fits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\R\model_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\R\experiment_1\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38821AB1-AC08-4765-BF10-A366A0ECE52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24CD28F-242E-44EC-BCAF-92218EACFF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{FF7DCB27-94D0-400E-979E-C88FDB044B91}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="16">
   <si>
     <t>participant</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>rho</t>
+  </si>
+  <si>
+    <t>Simultaneous</t>
+  </si>
+  <si>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>cond</t>
   </si>
 </sst>
 </file>
@@ -610,15 +619,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8EE00D-F6F0-44B3-A3B3-43FFBA811B96}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:E38"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,8 +643,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -651,8 +663,11 @@
       <c r="E2">
         <v>7.5379503771165396E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -668,8 +683,11 @@
       <c r="E3">
         <v>0.79972492943912399</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -685,8 +703,11 @@
       <c r="E4">
         <v>0.61105675012425498</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -702,8 +723,11 @@
       <c r="E5">
         <v>0.56560974648780005</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -719,8 +743,11 @@
       <c r="E6">
         <v>0.56707820795597297</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -736,8 +763,11 @@
       <c r="E7">
         <v>0.121494027333872</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -753,8 +783,11 @@
       <c r="E8">
         <v>0.67701082171307103</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -770,8 +803,11 @@
       <c r="E9">
         <v>0.47163106745522099</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -787,8 +823,11 @@
       <c r="E10">
         <v>0.472221439263729</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -804,8 +843,11 @@
       <c r="E11">
         <v>0.76029367986407403</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -821,8 +863,11 @@
       <c r="E12">
         <v>0.42883773461633901</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -838,8 +883,11 @@
       <c r="E13">
         <v>0.728225754931627</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -855,8 +903,11 @@
       <c r="E14">
         <v>0.766062268735059</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -872,8 +923,11 @@
       <c r="E15">
         <v>0.99267679020354505</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -889,8 +943,11 @@
       <c r="E16">
         <v>0.80129667989141495</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -906,8 +963,11 @@
       <c r="E17">
         <v>0.49759238515674098</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -923,8 +983,11 @@
       <c r="E18">
         <v>0.53914330225462104</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -940,8 +1003,11 @@
       <c r="E19">
         <v>6.2482839907604198E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -957,8 +1023,11 @@
       <c r="E20">
         <v>0.58085630454230497</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -974,8 +1043,11 @@
       <c r="E21">
         <v>0.57841411813791199</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -991,8 +1063,11 @@
       <c r="E22">
         <v>0.80501271999130697</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1008,8 +1083,11 @@
       <c r="E23">
         <v>0.882569560095122</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1025,8 +1103,11 @@
       <c r="E24">
         <v>0.73165943854777704</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1042,8 +1123,11 @@
       <c r="E25">
         <v>0.71742523415686099</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1059,8 +1143,11 @@
       <c r="E26">
         <v>0.65865546345333803</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1076,8 +1163,11 @@
       <c r="E27">
         <v>0.31066247050079498</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1093,8 +1183,11 @@
       <c r="E28">
         <v>0.56975748064523501</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1110,8 +1203,11 @@
       <c r="E29">
         <v>0.82921796764941902</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1127,8 +1223,11 @@
       <c r="E30">
         <v>0.86694704233772701</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1144,8 +1243,11 @@
       <c r="E31">
         <v>0.91588687998227203</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1161,8 +1263,11 @@
       <c r="E32">
         <v>0.238052295450528</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1178,8 +1283,11 @@
       <c r="E33">
         <v>0.74574852559233595</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1195,8 +1303,11 @@
       <c r="E34">
         <v>0.67600588703158804</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1212,8 +1323,11 @@
       <c r="E35">
         <v>0.440231756456054</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1229,8 +1343,11 @@
       <c r="E36">
         <v>0.63756651363461103</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1246,8 +1363,11 @@
       <c r="E37">
         <v>0.63285262947000198</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>18597.386239545198</v>
@@ -1272,15 +1392,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7809603-7B80-403B-ACE2-22F4CBF1A170}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:E38"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1296,8 +1416,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1313,8 +1436,11 @@
       <c r="E2">
         <v>6.9206455114307994E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1330,8 +1456,11 @@
       <c r="E3">
         <v>0.490465912136265</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1347,8 +1476,11 @@
       <c r="E4">
         <v>0.47633276700684801</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1364,8 +1496,11 @@
       <c r="E5">
         <v>0.46708917267802602</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1381,8 +1516,11 @@
       <c r="E6">
         <v>0.47845294941389499</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1398,8 +1536,11 @@
       <c r="E7">
         <v>9.8261339030729894E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1415,8 +1556,11 @@
       <c r="E8">
         <v>0.54808934333674397</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1432,8 +1576,11 @@
       <c r="E9">
         <v>0.39244567661630098</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1449,8 +1596,11 @@
       <c r="E10">
         <v>0.39616171328265398</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1466,8 +1616,11 @@
       <c r="E11">
         <v>0.69918211216675097</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1483,8 +1636,11 @@
       <c r="E12">
         <v>0.35661342549047897</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1500,8 +1656,11 @@
       <c r="E13">
         <v>0.25743552189664598</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1517,8 +1676,11 @@
       <c r="E14">
         <v>6.9408558674867504E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1534,8 +1696,11 @@
       <c r="E15">
         <v>0.98729802775116904</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1551,8 +1716,11 @@
       <c r="E16">
         <v>0.50857702925010795</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1568,8 +1736,11 @@
       <c r="E17">
         <v>0.44130687998144702</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1585,8 +1756,11 @@
       <c r="E18">
         <v>0.47863400325423699</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1602,8 +1776,11 @@
       <c r="E19">
         <v>5.5705470771703E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1619,8 +1796,11 @@
       <c r="E20">
         <v>0.468323344143665</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1636,8 +1816,11 @@
       <c r="E21">
         <v>0.47978422339641202</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1653,8 +1836,11 @@
       <c r="E22">
         <v>0.75010043638729795</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1670,8 +1856,11 @@
       <c r="E23">
         <v>0.80385844597588396</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1687,8 +1876,11 @@
       <c r="E24">
         <v>0.66153274135736095</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1704,8 +1896,11 @@
       <c r="E25">
         <v>0.64702393173795902</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1721,8 +1916,11 @@
       <c r="E26">
         <v>0.52402952067122699</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1738,8 +1936,11 @@
       <c r="E27">
         <v>0.28404720441133102</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1755,8 +1956,11 @@
       <c r="E28">
         <v>0.42256009592253102</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1772,8 +1976,11 @@
       <c r="E29">
         <v>0.66202899904482204</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1789,8 +1996,11 @@
       <c r="E30">
         <v>0.46697533580216799</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1806,8 +2016,11 @@
       <c r="E31">
         <v>0.70200963345650602</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1823,8 +2036,11 @@
       <c r="E32">
         <v>0.197323104913154</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1840,8 +2056,11 @@
       <c r="E33">
         <v>0.60790620829309305</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1857,8 +2076,11 @@
       <c r="E34">
         <v>0.42948398153852801</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1874,8 +2096,11 @@
       <c r="E35">
         <v>0.373591366641498</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1891,8 +2116,11 @@
       <c r="E36">
         <v>0.447786034207796</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1908,8 +2136,11 @@
       <c r="E37">
         <v>0.47250294146584398</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>19017.037350876646</v>
@@ -1934,15 +2165,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB00A94-EA9F-49FA-8DB8-C75B6170B57F}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1961,8 +2192,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1981,8 +2215,11 @@
       <c r="F2">
         <v>3.9174262797258698E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2001,8 +2238,11 @@
       <c r="F3">
         <v>0.71347760166069196</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2021,8 +2261,11 @@
       <c r="F4">
         <v>0.55727720360807398</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2041,8 +2284,11 @@
       <c r="F5">
         <v>0.38914837922594397</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2061,8 +2307,11 @@
       <c r="F6">
         <v>0.344529062998644</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2081,8 +2330,11 @@
       <c r="F7">
         <v>0.11306892984684</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2101,8 +2353,11 @@
       <c r="F8">
         <v>0.42688877606030301</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2121,8 +2376,11 @@
       <c r="F9">
         <v>0.28997611784479599</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2141,8 +2399,11 @@
       <c r="F10">
         <v>0.33110285213275897</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2161,8 +2422,11 @@
       <c r="F11">
         <v>0.40203594706071899</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2181,8 +2445,11 @@
       <c r="F12">
         <v>0.26199259360820698</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2201,8 +2468,11 @@
       <c r="F13">
         <v>0.66649778598826603</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2221,8 +2491,11 @@
       <c r="F14">
         <v>0.75507438362303103</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2241,8 +2514,11 @@
       <c r="F15">
         <v>0.65322937756652999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2261,8 +2537,11 @@
       <c r="F16">
         <v>0.76307357815659804</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2281,8 +2560,11 @@
       <c r="F17">
         <v>0.35270089179330899</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2301,8 +2583,11 @@
       <c r="F18">
         <v>0.34059765401713599</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2321,8 +2606,11 @@
       <c r="F19">
         <v>5.3497365490492402E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2341,8 +2629,11 @@
       <c r="F20">
         <v>0.35534394407442799</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2361,8 +2652,11 @@
       <c r="F21">
         <v>0.34944772466552898</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2381,8 +2675,11 @@
       <c r="F22">
         <v>0.41529747329161998</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2401,8 +2698,11 @@
       <c r="F23">
         <v>0.55098665042974704</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2421,8 +2721,11 @@
       <c r="F24">
         <v>0.410712538132111</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2441,8 +2744,11 @@
       <c r="F25">
         <v>0.37844512337666603</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2461,8 +2767,11 @@
       <c r="F26">
         <v>0.58047173923647499</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2481,8 +2790,11 @@
       <c r="F27">
         <v>0.164478735915598</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2501,8 +2813,11 @@
       <c r="F28">
         <v>0.55965559651502195</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2521,8 +2836,11 @@
       <c r="F29">
         <v>0.66719439178899997</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2541,8 +2859,11 @@
       <c r="F30">
         <v>0.77052770664123804</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2561,8 +2882,11 @@
       <c r="F31">
         <v>0.69171757416799096</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2581,8 +2905,11 @@
       <c r="F32">
         <v>0.140772884758362</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2601,8 +2928,11 @@
       <c r="F33">
         <v>0.58383234554631103</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2621,8 +2951,11 @@
       <c r="F34">
         <v>0.66605362868455598</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2641,8 +2974,11 @@
       <c r="F35">
         <v>0.39464482893759001</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2661,8 +2997,11 @@
       <c r="F36">
         <v>0.53618171921871305</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2681,8 +3020,11 @@
       <c r="F37">
         <v>0.57299241942452495</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>18422.95370666193</v>
@@ -2711,15 +3053,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C4DBFF-A6D5-41E3-8CE2-A4FFE426902D}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:G38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2741,8 +3083,11 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2764,8 +3109,11 @@
       <c r="G2">
         <v>5.0000000000936802E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2787,8 +3135,11 @@
       <c r="G3">
         <v>5.5432521973788E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2810,8 +3161,11 @@
       <c r="G4">
         <v>0.55750330967500406</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2833,8 +3187,11 @@
       <c r="G5">
         <v>0.44572612935836398</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2856,8 +3213,11 @@
       <c r="G6">
         <v>0.358259269559697</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2879,8 +3239,11 @@
       <c r="G7">
         <v>7.1671108367129699E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2902,8 +3265,11 @@
       <c r="G8">
         <v>0.40941994226513601</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2925,8 +3291,11 @@
       <c r="G9">
         <v>0.25127397531161799</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2948,8 +3317,11 @@
       <c r="G10">
         <v>0.32932906289387398</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2971,8 +3343,11 @@
       <c r="G11">
         <v>0.29755032647437102</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2994,8 +3369,11 @@
       <c r="G12">
         <v>5.0000000413178702E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3017,8 +3395,11 @@
       <c r="G13">
         <v>0.64888123221412797</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3040,8 +3421,11 @@
       <c r="G14">
         <v>0.71604489014089601</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3063,8 +3447,11 @@
       <c r="G15">
         <v>0.64554956160799204</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3086,8 +3473,11 @@
       <c r="G16">
         <v>5.0003490960625903E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3109,8 +3499,11 @@
       <c r="G17">
         <v>0.32531619475590301</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3132,8 +3525,11 @@
       <c r="G18">
         <v>0.270301605873978</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3155,8 +3551,11 @@
       <c r="G19">
         <v>5.0000000000606698E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3178,8 +3577,11 @@
       <c r="G20">
         <v>0.35200290516189903</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3201,8 +3603,11 @@
       <c r="G21">
         <v>0.31442773254691497</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3224,8 +3629,11 @@
       <c r="G22">
         <v>0.41367537043666702</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3247,8 +3655,11 @@
       <c r="G23">
         <v>0.51826110337006304</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3270,8 +3681,11 @@
       <c r="G24">
         <v>0.36940095238315601</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3293,8 +3707,11 @@
       <c r="G25">
         <v>0.26823021668474001</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3316,8 +3733,11 @@
       <c r="G26">
         <v>0.580282675006486</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3339,8 +3759,11 @@
       <c r="G27">
         <v>5.0000000001092698E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3362,8 +3785,11 @@
       <c r="G28">
         <v>0.19651538530749599</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3385,8 +3811,11 @@
       <c r="G29">
         <v>0.66818983731691906</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3408,8 +3837,11 @@
       <c r="G30">
         <v>0.77069358719451697</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3431,8 +3863,11 @@
       <c r="G31">
         <v>0.68774055575431203</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3454,8 +3889,11 @@
       <c r="G32">
         <v>0.15089704099047299</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3477,8 +3915,11 @@
       <c r="G33">
         <v>0.59511204374709503</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3500,8 +3941,11 @@
       <c r="G34">
         <v>5.0000000111985597E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3523,8 +3967,11 @@
       <c r="G35">
         <v>0.37408847179159599</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3546,8 +3993,11 @@
       <c r="G36">
         <v>0.55169988054340902</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3569,8 +4019,11 @@
       <c r="G37">
         <v>0.57532545545845504</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>18406.256780138447</v>
@@ -3603,15 +4056,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D84FD42-A03F-4259-8797-924A42D3EDEE}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:J38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3642,8 +4095,11 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3674,8 +4130,11 @@
       <c r="J2">
         <v>3.7062467308679098E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3706,8 +4165,11 @@
       <c r="J3">
         <v>0.311487042264109</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3738,8 +4200,11 @@
       <c r="J4">
         <v>0.51858279472648905</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3770,8 +4235,11 @@
       <c r="J5">
         <v>0.42344372346710701</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3802,8 +4270,11 @@
       <c r="J6">
         <v>0.34271902975785701</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3834,8 +4305,11 @@
       <c r="J7" s="1">
         <v>2.5410205711966E-7</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3866,8 +4340,11 @@
       <c r="J8">
         <v>0.422788285170208</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3898,8 +4375,11 @@
       <c r="J9">
         <v>0.24560069434086301</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3930,8 +4410,11 @@
       <c r="J10">
         <v>0.30207212511424197</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3962,8 +4445,11 @@
       <c r="J11">
         <v>0.41871144683953199</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3994,8 +4480,11 @@
       <c r="J12">
         <v>4.1862512282733001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4026,8 +4515,11 @@
       <c r="J13">
         <v>0.297402404169957</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4058,8 +4550,11 @@
       <c r="J14">
         <v>0.33372916747625903</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4090,8 +4585,11 @@
       <c r="J15">
         <v>0.89158396091915604</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4122,8 +4620,11 @@
       <c r="J16">
         <v>0.67544163321858197</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4154,8 +4655,11 @@
       <c r="J17">
         <v>0.297760679796224</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4186,8 +4690,11 @@
       <c r="J18">
         <v>0.35983121763005099</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4218,8 +4725,11 @@
       <c r="J19">
         <v>1.7930215002882399E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4250,8 +4760,11 @@
       <c r="J20">
         <v>0.36093039598109999</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4282,8 +4795,11 @@
       <c r="J21">
         <v>0.29584799560597602</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4314,8 +4830,11 @@
       <c r="J22">
         <v>0.41254670033854102</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4346,8 +4865,11 @@
       <c r="J23">
         <v>0.58604519602432503</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4378,8 +4900,11 @@
       <c r="J24">
         <v>0.39528024839866199</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4410,8 +4935,11 @@
       <c r="J25">
         <v>0.38462481075461602</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4442,8 +4970,11 @@
       <c r="J26">
         <v>0.51200640230254502</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4474,8 +5005,11 @@
       <c r="J27">
         <v>1.0230223924925E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4506,8 +5040,11 @@
       <c r="J28">
         <v>0.55073250692789499</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4538,8 +5075,11 @@
       <c r="J29">
         <v>0.72187550486437502</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4570,8 +5110,11 @@
       <c r="J30">
         <v>0.58237678168969098</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4602,8 +5145,11 @@
       <c r="J31">
         <v>0.77921349967508902</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4634,8 +5180,11 @@
       <c r="J32">
         <v>0.13784010326271101</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4666,8 +5215,11 @@
       <c r="J33">
         <v>0.58111360103370602</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4698,8 +5250,11 @@
       <c r="J34">
         <v>0.50228370270691503</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4730,8 +5285,11 @@
       <c r="J35">
         <v>0.25402254880557701</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4762,8 +5320,11 @@
       <c r="J36">
         <v>0.540774497205458</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4794,8 +5355,11 @@
       <c r="J37">
         <v>0.53185726827547597</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>18336.407961419907</v>
@@ -4840,15 +5404,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446D4221-8690-410F-9C37-DA1496246D3D}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:L38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4885,8 +5449,11 @@
       <c r="L1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4923,8 +5490,11 @@
       <c r="L2">
         <v>0.45258420030306601</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4961,8 +5531,11 @@
       <c r="L3">
         <v>0.62452736106458195</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4999,8 +5572,11 @@
       <c r="L4">
         <v>0.119645398468515</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5037,8 +5613,11 @@
       <c r="L5">
         <v>0.912181100651832</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5075,8 +5654,11 @@
       <c r="L6">
         <v>0.78236135704030096</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5113,8 +5695,11 @@
       <c r="L7">
         <v>0.75474634026505505</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5151,8 +5736,11 @@
       <c r="L8">
         <v>0.90384978510344705</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5189,8 +5777,11 @@
       <c r="L9">
         <v>0.90114286949759104</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5227,8 +5818,11 @@
       <c r="L10">
         <v>0.60081523008981197</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5265,8 +5859,11 @@
       <c r="L11">
         <v>0.56203422453822005</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5303,8 +5900,11 @@
       <c r="L12">
         <v>0.68908705843623497</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5341,8 +5941,11 @@
       <c r="L13">
         <v>0.204756375402212</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5379,8 +5982,11 @@
       <c r="L14">
         <v>0.55374870158940404</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5417,8 +6023,11 @@
       <c r="L15">
         <v>0.99304814756065596</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5455,8 +6064,11 @@
       <c r="L16">
         <v>1.25641089331628E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5493,8 +6105,11 @@
       <c r="L17">
         <v>0.64158938283696398</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5531,8 +6146,11 @@
       <c r="L18">
         <v>0.53938244301816396</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5569,8 +6187,11 @@
       <c r="L19">
         <v>0.99248581786388601</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5607,8 +6228,11 @@
       <c r="L20">
         <v>0.94309479029907495</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5645,8 +6269,11 @@
       <c r="L21">
         <v>0.89039201991781602</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5683,8 +6310,11 @@
       <c r="L22">
         <v>0.85320560270919799</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5721,8 +6351,11 @@
       <c r="L23">
         <v>0.57341226573555404</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5759,8 +6392,11 @@
       <c r="L24">
         <v>0.95116432917647997</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5797,8 +6433,11 @@
       <c r="L25">
         <v>0.87971399385081905</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5835,8 +6474,11 @@
       <c r="L26">
         <v>0.15714866532316399</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5873,8 +6515,11 @@
       <c r="L27">
         <v>0.35249770413673498</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5911,8 +6556,11 @@
       <c r="L28">
         <v>0.87629519347101403</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5949,8 +6597,11 @@
       <c r="L29">
         <v>0.86254356713951197</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5987,8 +6638,11 @@
       <c r="L30">
         <v>0.59803238002034198</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6025,8 +6679,11 @@
       <c r="L31">
         <v>0.46629062225392398</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6063,8 +6720,11 @@
       <c r="L32">
         <v>0.636249642989696</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6101,8 +6761,11 @@
       <c r="L33">
         <v>0.617256054133279</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6139,8 +6802,11 @@
       <c r="L34">
         <v>0.81854356154919194</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6177,8 +6843,11 @@
       <c r="L35">
         <v>0.27132112463004898</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6215,8 +6884,11 @@
       <c r="L36">
         <v>0.80484361404857796</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6253,8 +6925,11 @@
       <c r="L37">
         <v>2.3230419030528599E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B38">
         <f>SUM(B2:B37)</f>
         <v>18294.839674359737</v>

</xml_diff>